<commit_message>
fetch data from excel file with different templates along with multiple To and CC comma [,] separated
</commit_message>
<xml_diff>
--- a/src/resources/emp_det.xlsx
+++ b/src/resources/emp_det.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonkumar\IdeaProjects\HappyBirthday\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B45862-F928-404F-A26A-37BDF84199C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAE2AC0-E040-40E3-8176-1181ED638B5B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7360" xr2:uid="{170994D3-44A7-4659-8400-0BE51BE8C1A9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{170994D3-44A7-4659-8400-0BE51BE8C1A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Email_Id</t>
-  </si>
-  <si>
     <t>Srum</t>
   </si>
   <si>
@@ -57,15 +54,9 @@
     <t>Priyanshu Sadwal</t>
   </si>
   <si>
-    <t>Ap@gmail.com</t>
-  </si>
-  <si>
     <t>S@gmail.com</t>
   </si>
   <si>
-    <t>pubg57272@gmail.com</t>
-  </si>
-  <si>
     <t>Oncilla</t>
   </si>
   <si>
@@ -82,13 +73,34 @@
   </si>
   <si>
     <t>src\resources\template\template1.html</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>bcd@gmail.com</t>
+  </si>
+  <si>
+    <t>def@gmail.com</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Ap@gmail.com,abc@gmail.com</t>
+  </si>
+  <si>
+    <t>pubg57272@gmail.com,abc@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,12 +112,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,10 +138,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -451,92 +458,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E31DB9-3C4A-464D-B03D-E89C3DB310EB}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="22.26953125" customWidth="1"/>
-    <col min="5" max="5" width="47.36328125" customWidth="1"/>
+    <col min="1" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="38.08984375" customWidth="1"/>
+    <col min="6" max="6" width="47.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44094</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44095</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1">
-        <v>44082</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44096</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="1">
-        <v>44085</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1">
-        <v>44091</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{4CD8D02C-24A5-4763-B756-7284362CC521}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{4CD8D02C-24A5-4763-B756-7284362CC521}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{007D9838-1BC6-41EC-BC68-9AA485D2B023}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>